<commit_message>
Se corrigio nombres de los alumnos
</commit_message>
<xml_diff>
--- a/CASOS_DE_PRUEBA.xlsx
+++ b/CASOS_DE_PRUEBA.xlsx
@@ -39,39 +39,21 @@
     <t>Guillermo</t>
   </si>
   <si>
-    <t>Torres</t>
-  </si>
-  <si>
     <t>Stefania</t>
   </si>
   <si>
-    <t>Aczin</t>
-  </si>
-  <si>
     <t>Victoria</t>
   </si>
   <si>
-    <t>Finella</t>
-  </si>
-  <si>
     <t>Camila</t>
   </si>
   <si>
-    <t>Serfatti</t>
-  </si>
-  <si>
     <t>Santiago</t>
   </si>
   <si>
-    <t>Alaniz Pereyra</t>
-  </si>
-  <si>
     <t>Karim</t>
   </si>
   <si>
-    <t>Losada</t>
-  </si>
-  <si>
     <t>Agustina</t>
   </si>
   <si>
@@ -97,14 +79,40 @@
   </si>
   <si>
     <t>FINAL</t>
+  </si>
+  <si>
+    <t>Acziendo</t>
+  </si>
+  <si>
+    <t>Torreta</t>
+  </si>
+  <si>
+    <t>Finolla</t>
+  </si>
+  <si>
+    <t>Serf</t>
+  </si>
+  <si>
+    <t>Pirez</t>
+  </si>
+  <si>
+    <t>Luciendo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +449,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -483,15 +492,15 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -500,15 +509,15 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -517,15 +526,15 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -534,15 +543,15 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -551,15 +560,15 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -568,15 +577,15 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -585,15 +594,15 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
+      <c r="A9" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -602,14 +611,15 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Validacion de nombres y colores al grafico
</commit_message>
<xml_diff>
--- a/CASOS_DE_PRUEBA.xlsx
+++ b/CASOS_DE_PRUEBA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>APELLIDO</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Luciendo</t>
+  </si>
+  <si>
+    <t>FIN DEL PROGRAMA</t>
   </si>
 </sst>
 </file>
@@ -161,8 +164,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="APELLIDO"/>
     <tableColumn id="2" name="NOMBRE"/>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +617,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrego mensajes-guia y validar multiples apellidos
</commit_message>
<xml_diff>
--- a/CASOS_DE_PRUEBA.xlsx
+++ b/CASOS_DE_PRUEBA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>APELLIDO</t>
   </si>
@@ -100,22 +100,20 @@
   </si>
   <si>
     <t>FIN DEL PROGRAMA</t>
+  </si>
+  <si>
+    <t>De la Cruz</t>
+  </si>
+  <si>
+    <t>Esteban</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -145,7 +143,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,8 +162,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="APELLIDO"/>
     <tableColumn id="2" name="NOMBRE"/>
@@ -177,8 +175,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G1:G10" totalsRowShown="0">
-  <autoFilter ref="G1:G10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G1:G11" totalsRowShown="0">
+  <autoFilter ref="G1:G11"/>
   <tableColumns count="1">
     <tableColumn id="1" name="RESULTADOS ESPERADOS"/>
   </tableColumns>
@@ -449,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +616,27 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>